<commit_message>
Fixed DRC erros in layout, changed final BOM
</commit_message>
<xml_diff>
--- a/Kicad files/OpenHVPS-4/SEEED BOM.xlsx
+++ b/Kicad files/OpenHVPS-4/SEEED BOM.xlsx
@@ -20,39 +20,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="111">
   <si>
     <t xml:space="preserve">Designator</t>
   </si>
   <si>
-    <t xml:space="preserve">MPN/Seeed SKU</t>
+    <t xml:space="preserve">MPN</t>
   </si>
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
   <si>
+    <t xml:space="preserve">value</t>
+  </si>
+  <si>
     <t xml:space="preserve">Link</t>
   </si>
   <si>
-    <t xml:space="preserve">value</t>
-  </si>
-  <si>
     <t xml:space="preserve">C1</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacitor_SMD:C_0805_2012Metric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/885012207111/9346002</t>
-  </si>
-  <si>
     <t xml:space="preserve">150pF</t>
   </si>
   <si>
     <t xml:space="preserve">C2, C5, C10</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21B105KOFNNNG/3894469</t>
+    <t xml:space="preserve">CL21B105KOFNNNG</t>
   </si>
   <si>
     <t xml:space="preserve">1uF</t>
@@ -61,7 +55,7 @@
     <t xml:space="preserve">C3, C15</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/tdk-corporation/C1005X7R1H102K050BA/513719</t>
+    <t xml:space="preserve">C1005X7R1H102K050BA</t>
   </si>
   <si>
     <t xml:space="preserve">1nF</t>
@@ -70,10 +64,7 @@
     <t xml:space="preserve">C4</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacitor_SMD:C_1210_3225Metric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/taiyo-yuden/EMK325BJ106KN-T/930729</t>
+    <t xml:space="preserve">EMK325BJ106KN-T</t>
   </si>
   <si>
     <t xml:space="preserve">10uF</t>
@@ -82,7 +73,7 @@
     <t xml:space="preserve">C6, C7, C8, C9, C11, C12, C13, C14, C16, C17, C18, C19, C20, C21</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/tdk-corporation/C2012X7T2E104K125AA/2733184</t>
+    <t xml:space="preserve">C2012X7T2E104K125AA</t>
   </si>
   <si>
     <t xml:space="preserve">0.1uF</t>
@@ -91,7 +82,7 @@
     <t xml:space="preserve">C22</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/kemet/C0805C361J1GAC7800/2212653</t>
+    <t xml:space="preserve">C0805C361J1GAC7800</t>
   </si>
   <si>
     <t xml:space="preserve">360pF</t>
@@ -100,42 +91,36 @@
     <t xml:space="preserve">D1, D2</t>
   </si>
   <si>
-    <t xml:space="preserve">Diode_SMD:D_SOT-23_ANK</t>
+    <t xml:space="preserve">1N4148W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAS16</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.vishay.com/docs/85748/1n4148w.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">BAS16</t>
-  </si>
-  <si>
     <t xml:space="preserve">D3, D4, D5, D6, D7, D8, D9</t>
   </si>
   <si>
-    <t xml:space="preserve">Package_TO_SOT_SMD:SOT-23</t>
-  </si>
-  <si>
     <t xml:space="preserve">BAV23</t>
   </si>
   <si>
     <t xml:space="preserve">FB1, FB2</t>
   </si>
   <si>
-    <t xml:space="preserve">Resistor_SMD:R_0805_2012Metric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/taiyo-yuden/BKP2125HS221-T/957823</t>
-  </si>
-  <si>
     <t xml:space="preserve">BKP2125HS221-T</t>
   </si>
   <si>
+    <t xml:space="preserve">FI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRG21BC0R2MM1RA</t>
+  </si>
+  <si>
     <t xml:space="preserve">H1</t>
   </si>
   <si>
-    <t xml:space="preserve">TestPoint:TestPoint_Loop_D3.80mm_Drill2.0mm</t>
-  </si>
-  <si>
     <t xml:space="preserve">~</t>
   </si>
   <si>
@@ -151,37 +136,22 @@
     <t xml:space="preserve">J1, J2</t>
   </si>
   <si>
-    <t xml:space="preserve">Connector_PinHeader_2.54mm:PinHeader_1x03_P2.54mm_Vertical</t>
-  </si>
-  <si>
     <t xml:space="preserve">Conn_01x03_Male</t>
   </si>
   <si>
     <t xml:space="preserve">JP1</t>
   </si>
   <si>
-    <t xml:space="preserve">Jumper:SolderJumper-2_P1.3mm_Open_RoundedPad1.0x1.5mm</t>
-  </si>
-  <si>
     <t xml:space="preserve">L1</t>
   </si>
   <si>
-    <t xml:space="preserve">Inductor_SMD:L_Taiyo-Yuden_MD-4040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/taiyo-yuden/NRS6020T2R2NMGJ/2665967</t>
-  </si>
-  <si>
     <t xml:space="preserve">NRS6020T2R2NMGJ</t>
   </si>
   <si>
     <t xml:space="preserve">Q1</t>
   </si>
   <si>
-    <t xml:space="preserve">Package_TO_SOT_SMD:SOT-223-3_TabPin2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/on-semiconductor/FQT7N10LTF/965354</t>
+    <t xml:space="preserve">FQT7N10LTF</t>
   </si>
   <si>
     <t xml:space="preserve">FQT7N10</t>
@@ -190,7 +160,7 @@
     <t xml:space="preserve">Q2</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/diodes-incorporated/BC846A-7-F/1934446</t>
+    <t xml:space="preserve">BC846A-7-F</t>
   </si>
   <si>
     <t xml:space="preserve">BC846A</t>
@@ -199,10 +169,7 @@
     <t xml:space="preserve">Q3</t>
   </si>
   <si>
-    <t xml:space="preserve">Package_TO_SOT_SMD:SOT-363_SC-70-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/diodes-incorporated/MMDT3906-7-F/814540</t>
+    <t xml:space="preserve">MMDT3906-7-F</t>
   </si>
   <si>
     <t xml:space="preserve">MMDT3906</t>
@@ -211,10 +178,7 @@
     <t xml:space="preserve">R1, R2</t>
   </si>
   <si>
-    <t xml:space="preserve">Resistor_SMD:R_1206_3216Metric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RC1206FR-0710ML/728484</t>
+    <t xml:space="preserve">RC1206FR-0710ML</t>
   </si>
   <si>
     <t xml:space="preserve">10M</t>
@@ -223,7 +187,7 @@
     <t xml:space="preserve">R3, R4</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805FT100K/1760712</t>
+    <t xml:space="preserve">RMCF0805FT100K</t>
   </si>
   <si>
     <t xml:space="preserve">100K</t>
@@ -232,13 +196,13 @@
     <t xml:space="preserve">R5, R12</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/te-connectivity-passive-product/CRG0805F100R/2380830</t>
+    <t xml:space="preserve">CRG0805F100R</t>
   </si>
   <si>
     <t xml:space="preserve">R6</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/koa-speer-electronics-inc/RK73H2ATTD1213F/10235721</t>
+    <t xml:space="preserve">RK73H2ATTD1213F</t>
   </si>
   <si>
     <t xml:space="preserve">121k</t>
@@ -247,7 +211,7 @@
     <t xml:space="preserve">R7, R8, R9, R10</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805FT22M0/6053747</t>
+    <t xml:space="preserve">RMCF0805FT22M0</t>
   </si>
   <si>
     <t xml:space="preserve">22M</t>
@@ -256,7 +220,7 @@
     <t xml:space="preserve">R11</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/te-connectivity-passive-product/CRGCQ0805F33K/8576369</t>
+    <t xml:space="preserve">CRGCQ0805F33K</t>
   </si>
   <si>
     <t xml:space="preserve">33k</t>
@@ -271,7 +235,7 @@
     <t xml:space="preserve">R14</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/vishay-dale/CRCW08051M50FKEA/1176034</t>
+    <t xml:space="preserve">CRCW08051M50FKEA</t>
   </si>
   <si>
     <t xml:space="preserve">1M5</t>
@@ -280,7 +244,7 @@
     <t xml:space="preserve">R15</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RC0805FR-07392KL/727905</t>
+    <t xml:space="preserve">RC0805FR-07392KL</t>
   </si>
   <si>
     <t xml:space="preserve">392k</t>
@@ -289,7 +253,7 @@
     <t xml:space="preserve">R16</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RT0805FRE071ML/1079056</t>
+    <t xml:space="preserve">RT0805FRE071ML</t>
   </si>
   <si>
     <t xml:space="preserve">1M</t>
@@ -298,7 +262,7 @@
     <t xml:space="preserve">R17</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805FT499K/1760301</t>
+    <t xml:space="preserve">RMCF0805FT499K</t>
   </si>
   <si>
     <t xml:space="preserve">499k</t>
@@ -307,7 +271,7 @@
     <t xml:space="preserve">R18</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RT0805FRE071KL/1079055</t>
+    <t xml:space="preserve">RT0805FRE071KL</t>
   </si>
   <si>
     <t xml:space="preserve">1k</t>
@@ -316,7 +280,7 @@
     <t xml:space="preserve">R20</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RT0805FRE07560KL/1079317</t>
+    <t xml:space="preserve">RT0805FRE07560KL</t>
   </si>
   <si>
     <t xml:space="preserve">560K</t>
@@ -325,7 +289,7 @@
     <t xml:space="preserve">R21</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RC0805FR-0747KL/727973</t>
+    <t xml:space="preserve">RC0805FR-0747KL</t>
   </si>
   <si>
     <t xml:space="preserve">47k</t>
@@ -334,7 +298,7 @@
     <t xml:space="preserve">R22</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-6ENF2002V/111532</t>
+    <t xml:space="preserve">ERJ-6ENF2002V</t>
   </si>
   <si>
     <t xml:space="preserve">20k</t>
@@ -343,7 +307,7 @@
     <t xml:space="preserve">R23</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RC0805FR-073M16L/727809</t>
+    <t xml:space="preserve">RC0805FR-073M16L</t>
   </si>
   <si>
     <t xml:space="preserve">3.16M</t>
@@ -352,7 +316,7 @@
     <t xml:space="preserve">U1</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/maxim-integrated/MAX6008AEUR-T/1519060</t>
+    <t xml:space="preserve">MAX6008AEUR-T</t>
   </si>
   <si>
     <t xml:space="preserve">MAX6008AEUR+T</t>
@@ -361,10 +325,7 @@
     <t xml:space="preserve">U2</t>
   </si>
   <si>
-    <t xml:space="preserve">Package_SO:SOIC-14_3.9x8.7mm_P1.27mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/texas-instruments/CD74HC14M96/390309</t>
+    <t xml:space="preserve">CD74HC14M96</t>
   </si>
   <si>
     <t xml:space="preserve">74HC14</t>
@@ -373,25 +334,25 @@
     <t xml:space="preserve">U3</t>
   </si>
   <si>
-    <t xml:space="preserve">Package_TO_SOT_SMD:SOT-23-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.ti.com/lit/ds/symlink/tlv2375.pdf</t>
+    <t xml:space="preserve">TLV2375</t>
   </si>
   <si>
     <t xml:space="preserve">MAX4162</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.ti.com/lit/ds/symlink/tlv2375.pdf</t>
+  </si>
+  <si>
     <t xml:space="preserve">U4</t>
   </si>
   <si>
-    <t xml:space="preserve">Package_SO:SOIC-16_3.9x9.9mm_P1.27mm</t>
+    <t xml:space="preserve">HEF4538BT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD14538BM</t>
   </si>
   <si>
     <t xml:space="preserve">https://assets.nexperia.com/documents/data-sheet/HEF4538B.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD14538BM</t>
   </si>
 </sst>
 </file>
@@ -401,7 +362,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -430,6 +391,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -474,7 +441,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -484,11 +451,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -568,18 +543,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E38"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.078125" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="40.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="52.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="43.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -589,10 +565,10 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
@@ -603,632 +579,545 @@
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="n">
+        <v>885012207111</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="n">
         <v>14</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="0" t="s">
+      <c r="B8" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="C8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="E8" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="n">
         <v>7</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="C12" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>2</v>
+        <v>33</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>1</v>
+        <v>33</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>2</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="0" t="n">
-        <v>7317</v>
-      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>50</v>
+        <v>33</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>7317</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="C16" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="C17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="C18" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="0" t="n">
-        <v>2</v>
+        <v>49</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="C20" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="C21" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>100</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>73</v>
+        <v>58</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>4</v>
+        <v>60</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>4</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <v>2</v>
+        <v>66</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="0" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>2</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="C27" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="C28" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="C29" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="C30" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="C31" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="C32" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="C33" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="C34" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="C35" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C36" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="C36" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="C37" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="C37" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="C38" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="C38" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>123</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E8" r:id="rId1" display="https://www.vishay.com/docs/85748/1n4148w.pdf"/>
+    <hyperlink ref="E38" r:id="rId2" display="https://www"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>